<commit_message>
GUI: Stats updates JobStatus WIP
</commit_message>
<xml_diff>
--- a/QA/Tests/CRUD/Delete/_Test_Suite_Statistics.xlsx
+++ b/QA/Tests/CRUD/Delete/_Test_Suite_Statistics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Title</t>
   </si>
@@ -58,6 +58,9 @@
   </si>
   <si>
     <t>Suite to manual</t>
+  </si>
+  <si>
+    <t>Ready to write</t>
   </si>
 </sst>
 </file>
@@ -152,7 +155,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="24">
     <dxf>
       <fill>
         <patternFill>
@@ -210,73 +213,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill>
-          <stop position="0">
-            <color rgb="FF00B0F0"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <gradientFill degree="180">
-          <stop position="0">
-            <color rgb="FF66FF66"/>
-          </stop>
-          <stop position="1">
-            <color rgb="FF00B050"/>
-          </stop>
-        </gradientFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FF66FF66"/>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF66FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -729,7 +665,7 @@
   <dimension ref="A1:I175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -766,14 +702,14 @@
       </c>
       <c r="G1" s="6">
         <f>COUNTIF($D:$D,"Ready to Write")+COUNTIF($D:$D,"Outdated")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3">
         <f>SUM(G1:G2)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -787,10 +723,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>6</v>
@@ -808,7 +741,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>12</v>
@@ -825,7 +758,7 @@
       </c>
       <c r="G4" s="3">
         <f>SUM($C:$C)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -862,86 +795,86 @@
     <sortCondition ref="A2"/>
   </sortState>
   <conditionalFormatting sqref="D4:D51">
-    <cfRule type="notContainsBlanks" dxfId="31" priority="25" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="23" priority="25" stopIfTrue="1">
       <formula>LEN(TRIM(D4))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1 D4:D1048576">
-    <cfRule type="containsText" dxfId="30" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="22" priority="17" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="21" priority="18" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="28" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="20" priority="19" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="27" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="19" priority="20" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="18" priority="21" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="17" priority="22" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="16" priority="23" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="notContainsBlanks" dxfId="23" priority="16" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="15" priority="16" stopIfTrue="1">
       <formula>LEN(TRIM(D2))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2">
-    <cfRule type="containsText" dxfId="22" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="14" priority="9" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="13" priority="10" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="12" priority="11" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="11" priority="12" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="10" priority="13" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="17" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="9" priority="14" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="8" priority="15" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="notContainsBlanks" dxfId="15" priority="8" stopIfTrue="1">
+    <cfRule type="notContainsBlanks" dxfId="7" priority="8" stopIfTrue="1">
       <formula>LEN(TRIM(D3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D3">
-    <cfRule type="containsText" dxfId="13" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
+    <cfRule type="containsText" dxfId="6" priority="1" stopIfTrue="1" operator="containsText" text="Finished">
       <formula>NOT(ISERROR(SEARCH("Finished",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="12" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
+    <cfRule type="containsText" dxfId="5" priority="2" stopIfTrue="1" operator="containsText" text="Automated">
       <formula>NOT(ISERROR(SEARCH("Automated",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
+    <cfRule type="containsText" dxfId="4" priority="3" stopIfTrue="1" operator="containsText" text="Under Review">
       <formula>NOT(ISERROR(SEARCH("Under Review",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
+    <cfRule type="containsText" dxfId="3" priority="4" stopIfTrue="1" operator="containsText" text="Testing">
       <formula>NOT(ISERROR(SEARCH("Testing",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
+    <cfRule type="containsText" dxfId="2" priority="5" stopIfTrue="1" operator="containsText" text="Writing">
       <formula>NOT(ISERROR(SEARCH("Writing",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
+    <cfRule type="containsText" dxfId="1" priority="6" stopIfTrue="1" operator="containsText" text="Ready to Write">
       <formula>NOT(ISERROR(SEARCH("Ready to Write",D3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
+    <cfRule type="containsText" dxfId="0" priority="7" stopIfTrue="1" operator="containsText" text="Unwritten Keywords">
       <formula>NOT(ISERROR(SEARCH("Unwritten Keywords",D3)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>